<commit_message>
desarrollo de completado de formulario expedicion de poliza
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>MNY397</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Dirección</t>
   </si>
@@ -47,13 +45,124 @@
     <t>Placa</t>
   </si>
   <si>
-    <t>Calle123</t>
-  </si>
-  <si>
     <t>test@gmail.com</t>
   </si>
   <si>
     <t>RESIDENCIA</t>
+  </si>
+  <si>
+    <t>ENQ122</t>
+  </si>
+  <si>
+    <t>Tipo Identificacion</t>
+  </si>
+  <si>
+    <t>Número Identificación</t>
+  </si>
+  <si>
+    <t>Digito Identificación</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Tipo de Persona</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Tipo de Empresa</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>ASOCIACION</t>
+  </si>
+  <si>
+    <t>CONSORCIO</t>
+  </si>
+  <si>
+    <t>COOPERATIVAYPRECOOPERATIVA</t>
+  </si>
+  <si>
+    <t>EMPRESAASOCIATIVADETRABAJO</t>
+  </si>
+  <si>
+    <t>EMPRESAESTATAL</t>
+  </si>
+  <si>
+    <t>FONDODEEMPLEADOS</t>
+  </si>
+  <si>
+    <t>FUNDACION</t>
+  </si>
+  <si>
+    <t>JUNTASDEACCIONCOMUNAL</t>
+  </si>
+  <si>
+    <t>ORGANIZACIONNOGUBERNAMENTALONG</t>
+  </si>
+  <si>
+    <t>OTROS</t>
+  </si>
+  <si>
+    <t>S.A.SSOCIEDADESPORACCIONESSIMPLIFICADA</t>
+  </si>
+  <si>
+    <t>SINDICATO</t>
+  </si>
+  <si>
+    <t>SOCIEDADANONIMA</t>
+  </si>
+  <si>
+    <t>SOCIEDADCOLECTIVA</t>
+  </si>
+  <si>
+    <t>SOCIEDADDERESPONSABILIDADLTDA</t>
+  </si>
+  <si>
+    <t>SOCIEDADENCOMANDITAPORACCIONES</t>
+  </si>
+  <si>
+    <t>SOCIEDADENCOMANDITASIMPLE</t>
+  </si>
+  <si>
+    <t>SOCIEDADESDEECONOMIAMIXTA</t>
+  </si>
+  <si>
+    <t>SOCIEDADESDEHECHO</t>
+  </si>
+  <si>
+    <t>UNIONTEMPORAL</t>
+  </si>
+  <si>
+    <t>UNIPERSONAL</t>
+  </si>
+  <si>
+    <t>Ocupación - CIIU</t>
+  </si>
+  <si>
+    <t>1er. Apellido / Razón Social</t>
+  </si>
+  <si>
+    <t>2do. Apellido</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Tipo de Dirección</t>
+  </si>
+  <si>
+    <t>Calle 123</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Municipio</t>
   </si>
 </sst>
 </file>
@@ -383,70 +492,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>6664221</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>6664221</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="S2">
         <v>3054665663</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
       <formula1>"NA, BEEPER, CASA, CELULAR, E-MAIL, OFICINA, OFICINA 2, OFICINA 3, PBX / CONMUTADOR, RESIDENCIA, RESIDENCIA 2, TELEFAX, TELFAX 2, TRANSFERENCIAS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"NA,CEDULA DE CIUDADANIA, CEDULA DE EXTRANJERIA, NRO DE NIT, PASAPORTE, TARJETA DE IDENTIDAD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>"NA, MASCULINO, FEMENINO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>"NA,NATURAL,JURIDICA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+      <formula1>"NA,APARTADO AEREO, DOMICILIO, OFICINA/COMERCIAL, PRUEBA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="R2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja2!$A$2:$A$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B1:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicion de campo observacion
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -495,7 +495,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,21 +634,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
       <formula1>"NA, BEEPER, CASA, CELULAR, E-MAIL, OFICINA, OFICINA 2, OFICINA 3, PBX / CONMUTADOR, RESIDENCIA, RESIDENCIA 2, TELEFAX, TELFAX 2, TRANSFERENCIAS"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"NA,CEDULA DE CIUDADANIA, CEDULA DE EXTRANJERIA, NRO DE NIT, PASAPORTE, TARJETA DE IDENTIDAD"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>"NA, MASCULINO, FEMENINO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
-      <formula1>"NA,NATURAL,JURIDICA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
-      <formula1>"NA,APARTADO AEREO, DOMICILIO, OFICINA/COMERCIAL, PRUEBA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -656,18 +647,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Hoja2!$A$2:$A$24</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Estructuracion de reporte serenityReport
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\proyectos\segurosmundial\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\soat-web\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -162,14 +162,14 @@
     <t>Municipio</t>
   </si>
   <si>
-    <t>WFL326</t>
+    <t>AMZ45D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +184,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,10 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -495,7 +502,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +582,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B2" t="s">

</xml_diff>

<commit_message>
modificacion de url del aplicativo
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>Dirección</t>
   </si>
@@ -162,7 +162,16 @@
     <t>Municipio</t>
   </si>
   <si>
-    <t>AMZ45D</t>
+    <t>tes2t@gmail.com</t>
+  </si>
+  <si>
+    <t>Calle 1234</t>
+  </si>
+  <si>
+    <t>SZV190</t>
+  </si>
+  <si>
+    <t>GBL76F</t>
   </si>
 </sst>
 </file>
@@ -499,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +592,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -640,20 +649,80 @@
         <v>3054665663</v>
       </c>
     </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>6664331</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3">
+        <v>3054665669</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
       <formula1>"NA, BEEPER, CASA, CELULAR, E-MAIL, OFICINA, OFICINA 2, OFICINA 3, PBX / CONMUTADOR, RESIDENCIA, RESIDENCIA 2, TELEFAX, TELFAX 2, TRANSFERENCIAS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
       <formula1>"NA,CEDULA DE CIUDADANIA, CEDULA DE EXTRANJERIA, NRO DE NIT, PASAPORTE, TARJETA DE IDENTIDAD"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1"/>
+    <hyperlink ref="R3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modificacion de reporte serenity
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Dirección</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Placa</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
     <t>RESIDENCIA</t>
   </si>
   <si>
@@ -160,18 +157,6 @@
   </si>
   <si>
     <t>Municipio</t>
-  </si>
-  <si>
-    <t>tes2t@gmail.com</t>
-  </si>
-  <si>
-    <t>Calle 1234</t>
-  </si>
-  <si>
-    <t>SZV190</t>
-  </si>
-  <si>
-    <t>GBL76F</t>
   </si>
 </sst>
 </file>
@@ -510,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +514,7 @@
     <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -536,37 +522,37 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -578,10 +564,10 @@
         <v>2</v>
       </c>
       <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
       <c r="R1" t="s">
         <v>3</v>
@@ -591,122 +577,61 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O2">
         <v>6664221</v>
       </c>
       <c r="P2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2">
-        <v>3054665663</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3">
-        <v>6664331</v>
-      </c>
-      <c r="P3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3">
-        <v>3054665669</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="N3" s="2"/>
+      <c r="R3" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -717,12 +642,8 @@
       <formula1>"NA,CEDULA DE CIUDADANIA, CEDULA DE EXTRANJERIA, NRO DE NIT, PASAPORTE, TARJETA DE IDENTIDAD"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1"/>
-    <hyperlink ref="R3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -731,7 +652,7 @@
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B1:B37"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,122 +662,122 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificacion de valores en el documento excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Dirección</t>
   </si>
@@ -69,6 +69,96 @@
     <t>Tipo de Empresa</t>
   </si>
   <si>
+    <t>Ocupación - CIIU</t>
+  </si>
+  <si>
+    <t>1er. Apellido / Razón Social</t>
+  </si>
+  <si>
+    <t>2do. Apellido</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Tipo de Dirección</t>
+  </si>
+  <si>
+    <t>Calle 123</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Municipio</t>
+  </si>
+  <si>
+    <t>alba3.example@gmail.com</t>
+  </si>
+  <si>
+    <t>EYX488</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Linea</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Cilindraje</t>
+  </si>
+  <si>
+    <t>DATOS DEL VEHICULO</t>
+  </si>
+  <si>
+    <t>Pasajeros</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Chasis</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>Pais del Vehiculo</t>
+  </si>
+  <si>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>VEH. PARTICULARES 6 O MAS PASAJEROS</t>
+  </si>
+  <si>
+    <t>BYD</t>
+  </si>
+  <si>
+    <t>S6 GLX</t>
+  </si>
+  <si>
+    <t>PARTICULAR</t>
+  </si>
+  <si>
+    <t>CAXE11805</t>
+  </si>
+  <si>
+    <t>WAUZZZ8X4EB049715</t>
+  </si>
+  <si>
+    <t>DATOS DEL TOMADOR</t>
+  </si>
+  <si>
     <t>ADMINISTRADOR</t>
   </si>
   <si>
@@ -78,92 +168,104 @@
     <t>CONSORCIO</t>
   </si>
   <si>
-    <t>COOPERATIVAYPRECOOPERATIVA</t>
-  </si>
-  <si>
-    <t>EMPRESAASOCIATIVADETRABAJO</t>
-  </si>
-  <si>
-    <t>EMPRESAESTATAL</t>
-  </si>
-  <si>
-    <t>FONDODEEMPLEADOS</t>
+    <t>COOPERATIVA Y PRECOOPERATIVA</t>
+  </si>
+  <si>
+    <t>EMPRESA ASOCIATIVA DE TRABAJO</t>
+  </si>
+  <si>
+    <t>EMPRESA ESTATAL</t>
+  </si>
+  <si>
+    <t>FONDO DE EMPLEADOS</t>
   </si>
   <si>
     <t>FUNDACION</t>
   </si>
   <si>
-    <t>JUNTASDEACCIONCOMUNAL</t>
-  </si>
-  <si>
-    <t>ORGANIZACIONNOGUBERNAMENTALONG</t>
+    <t>JUNTAS DE ACCION COMUNAL</t>
+  </si>
+  <si>
+    <t>ORGANIZACION NO GUBERNAMENTAL ONG</t>
   </si>
   <si>
     <t>OTROS</t>
   </si>
   <si>
-    <t>S.A.SSOCIEDADESPORACCIONESSIMPLIFICADA</t>
+    <t>S.A.S SOCIEDADES POR ACCIONES SIMPLIFICADA</t>
   </si>
   <si>
     <t>SINDICATO</t>
   </si>
   <si>
-    <t>SOCIEDADANONIMA</t>
-  </si>
-  <si>
-    <t>SOCIEDADCOLECTIVA</t>
-  </si>
-  <si>
-    <t>SOCIEDADDERESPONSABILIDADLTDA</t>
-  </si>
-  <si>
-    <t>SOCIEDADENCOMANDITAPORACCIONES</t>
-  </si>
-  <si>
-    <t>SOCIEDADENCOMANDITASIMPLE</t>
-  </si>
-  <si>
-    <t>SOCIEDADESDEECONOMIAMIXTA</t>
-  </si>
-  <si>
-    <t>SOCIEDADESDEHECHO</t>
-  </si>
-  <si>
-    <t>UNIONTEMPORAL</t>
+    <t>SOCIEDAD ANONIMA</t>
+  </si>
+  <si>
+    <t>SOCIEDAD COLECTIVA</t>
+  </si>
+  <si>
+    <t>SOCIEDAD DE RESPONSABILIDAD LTDA</t>
+  </si>
+  <si>
+    <t>SOCIEDAD EN COMANDITA POR ACCIONES</t>
+  </si>
+  <si>
+    <t>SOCIEDAD EN COMANDITA SIMPLE</t>
+  </si>
+  <si>
+    <t>SOCIEDADES DE ECONOMIA MIXTA</t>
+  </si>
+  <si>
+    <t>SOCIEDADES DE HECHO</t>
+  </si>
+  <si>
+    <t>UNION TEMPORAL</t>
   </si>
   <si>
     <t>UNIPERSONAL</t>
   </si>
   <si>
-    <t>Ocupación - CIIU</t>
-  </si>
-  <si>
-    <t>1er. Apellido / Razón Social</t>
-  </si>
-  <si>
-    <t>2do. Apellido</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Tipo de Dirección</t>
-  </si>
-  <si>
-    <t>Calle 123</t>
-  </si>
-  <si>
-    <t>Departamento</t>
-  </si>
-  <si>
-    <t>Municipio</t>
+    <t>ACTIVIDADES AUXILIARES DE LOS SEGUROS</t>
+  </si>
+  <si>
+    <t>CEDULA DE CIUDADANIA</t>
+  </si>
+  <si>
+    <t>MASCULINO</t>
+  </si>
+  <si>
+    <t>NATURAL</t>
+  </si>
+  <si>
+    <t>Salinas</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>DOMICILIO</t>
+  </si>
+  <si>
+    <t>BOLIVAR</t>
+  </si>
+  <si>
+    <t>CARTAGENA</t>
+  </si>
+  <si>
+    <t>BRASIL</t>
+  </si>
+  <si>
+    <t>0.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,22 +283,85 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF202124"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -207,11 +372,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -228,6 +413,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:A25" totalsRowShown="0">
+  <autoFilter ref="A1:A25"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Tipo de Empresa"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,157 +688,836 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="21" max="21" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" customWidth="1"/>
+    <col min="30" max="30" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+    </row>
+    <row r="2" spans="1:31" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="O2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="P2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="T2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="F3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1390</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="2">
+        <v>73655423</v>
+      </c>
+      <c r="P3" s="2">
         <v>2</v>
       </c>
-      <c r="P1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O2">
+      <c r="AA3" s="2">
         <v>6664221</v>
       </c>
-      <c r="P2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="N3" s="2"/>
-      <c r="R3" s="1"/>
+      <c r="AB3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>3053776994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+    </row>
+    <row r="5" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+    </row>
+    <row r="6" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+    </row>
+    <row r="7" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+    </row>
+    <row r="8" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+    </row>
+    <row r="9" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+    </row>
+    <row r="10" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+    </row>
+    <row r="11" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+    </row>
+    <row r="12" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+    </row>
+    <row r="13" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+    </row>
+    <row r="14" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+    </row>
+    <row r="15" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+    </row>
+    <row r="16" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+    </row>
+    <row r="17" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+    </row>
+    <row r="18" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+    </row>
+    <row r="19" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
+  <mergeCells count="2">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="N1:AE1"/>
+  </mergeCells>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3">
       <formula1>"NA, BEEPER, CASA, CELULAR, E-MAIL, OFICINA, OFICINA 2, OFICINA 3, PBX / CONMUTADOR, RESIDENCIA, RESIDENCIA 2, TELEFAX, TELFAX 2, TRANSFERENCIAS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3">
       <formula1>"NA,CEDULA DE CIUDADANIA, CEDULA DE EXTRANJERIA, NRO DE NIT, PASAPORTE, TARJETA DE IDENTIDAD"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Selecciona una clase" sqref="B3">
+      <formula1>"NA,MOTOCICLETA,MOTO CARRO,CICLOMOTOR,CAMPEROS Y CAMIONETAS,CARGA O MIXTOS,OFICIALES ESPECIALES,AUTOMOVILES FAMILIARES,VEH. PARTICULARES 6 O MAS PASAJEROS,AUTOS DE NEGOCIO ALQUILER ENSEÐANZA,BUSES O BUSETAS,S. PUB. INTERMUNICIPAL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3">
+      <formula1>"NA,COLOMBIA,BRASIL,ECUADOR,VENEZUELA,PERU,PANAMA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3">
+      <formula1>"NA,MASCULINO,FEMENINO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3">
+      <formula1>"NA,NATURAL,JURIDICA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3">
+      <formula1>"NA,APARTADO AEREO,DOMICILIO,OFICINA/COMERCIAL,PRUEBA"</formula1>
+    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AD3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja2!$A$2:$A$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>S3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -652,12 +1526,12 @@
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -672,115 +1546,118 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>